<commit_message>
Last Commit before invited Mentors
</commit_message>
<xml_diff>
--- a/Eleves.xlsx
+++ b/Eleves.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="111">
   <si>
     <t>Nom</t>
   </si>
@@ -114,14 +114,265 @@
   </si>
   <si>
     <t>08/20</t>
+  </si>
+  <si>
+    <t>Ousmane</t>
+  </si>
+  <si>
+    <t>16/20</t>
+  </si>
+  <si>
+    <t>Fall</t>
+  </si>
+  <si>
+    <t>Dia</t>
+  </si>
+  <si>
+    <t>Mouhamed</t>
+  </si>
+  <si>
+    <t>Pikine</t>
+  </si>
+  <si>
+    <t>05/20</t>
+  </si>
+  <si>
+    <t>07/20</t>
+  </si>
+  <si>
+    <t>09/20</t>
+  </si>
+  <si>
+    <t>11/20</t>
+  </si>
+  <si>
+    <t>12/20</t>
+  </si>
+  <si>
+    <t>04/20</t>
+  </si>
+  <si>
+    <t>10/20</t>
+  </si>
+  <si>
+    <t>13/20</t>
+  </si>
+  <si>
+    <t>06/20</t>
+  </si>
+  <si>
+    <t>Saint-Louis</t>
+  </si>
+  <si>
+    <t>Thies</t>
+  </si>
+  <si>
+    <t>Matam</t>
+  </si>
+  <si>
+    <t>Louga</t>
+  </si>
+  <si>
+    <t>Diourbel</t>
+  </si>
+  <si>
+    <t>Kolda</t>
+  </si>
+  <si>
+    <t>Kaolack</t>
+  </si>
+  <si>
+    <t>Gueye</t>
+  </si>
+  <si>
+    <t>Gaye</t>
+  </si>
+  <si>
+    <t>Kane</t>
+  </si>
+  <si>
+    <t>Ly</t>
+  </si>
+  <si>
+    <t>Mané</t>
+  </si>
+  <si>
+    <t>Ndiaye</t>
+  </si>
+  <si>
+    <t>Ngom</t>
+  </si>
+  <si>
+    <t>Pouye</t>
+  </si>
+  <si>
+    <t>Séne</t>
+  </si>
+  <si>
+    <t>Thiam</t>
+  </si>
+  <si>
+    <t>Tiabou</t>
+  </si>
+  <si>
+    <t>Tiaw</t>
+  </si>
+  <si>
+    <t>Guédiawaye</t>
+  </si>
+  <si>
+    <t>Khor</t>
+  </si>
+  <si>
+    <t>Bargny</t>
+  </si>
+  <si>
+    <t>Mbour</t>
+  </si>
+  <si>
+    <t>Salam</t>
+  </si>
+  <si>
+    <t>Tiakhane</t>
+  </si>
+  <si>
+    <t>Randouléne</t>
+  </si>
+  <si>
+    <t>Yoro</t>
+  </si>
+  <si>
+    <t>HLM</t>
+  </si>
+  <si>
+    <t>Mamadou</t>
+  </si>
+  <si>
+    <t>Demba</t>
+  </si>
+  <si>
+    <t>Maty</t>
+  </si>
+  <si>
+    <t>Mariama</t>
+  </si>
+  <si>
+    <t>Abssa</t>
+  </si>
+  <si>
+    <t>Astou</t>
+  </si>
+  <si>
+    <t>Sidy</t>
+  </si>
+  <si>
+    <t>Khadim</t>
+  </si>
+  <si>
+    <t>Issa</t>
+  </si>
+  <si>
+    <t>Soulaymane</t>
+  </si>
+  <si>
+    <t>Pape</t>
+  </si>
+  <si>
+    <t>Amadou</t>
+  </si>
+  <si>
+    <t>Ibrahima</t>
+  </si>
+  <si>
+    <t>Mimy</t>
+  </si>
+  <si>
+    <t>Rosalie</t>
+  </si>
+  <si>
+    <t>Seune</t>
+  </si>
+  <si>
+    <t>Fatou</t>
+  </si>
+  <si>
+    <t>Fama</t>
+  </si>
+  <si>
+    <t>Aya</t>
+  </si>
+  <si>
+    <t>Sokhna</t>
+  </si>
+  <si>
+    <t>Arame</t>
+  </si>
+  <si>
+    <t>Abdou</t>
+  </si>
+  <si>
+    <t>Tapha</t>
+  </si>
+  <si>
+    <t>Mamy</t>
+  </si>
+  <si>
+    <t>Josephine</t>
+  </si>
+  <si>
+    <t>Marie</t>
+  </si>
+  <si>
+    <t>Saly</t>
+  </si>
+  <si>
+    <t>Oumou</t>
+  </si>
+  <si>
+    <t>Rokhaya</t>
+  </si>
+  <si>
+    <t>Gnagna</t>
+  </si>
+  <si>
+    <t>Awa</t>
+  </si>
+  <si>
+    <t>Mame Diara</t>
+  </si>
+  <si>
+    <t>Adji</t>
+  </si>
+  <si>
+    <t>Aïda</t>
+  </si>
+  <si>
+    <t>Fallou</t>
+  </si>
+  <si>
+    <t>Maïmouna</t>
+  </si>
+  <si>
+    <t>Comba</t>
+  </si>
+  <si>
+    <t>Alima</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -149,9 +400,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,40 +685,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="1"/>
     <col min="7" max="7" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -479,7 +734,7 @@
       <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E2">
@@ -505,7 +760,7 @@
       <c r="C3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E3">
@@ -531,7 +786,7 @@
       <c r="C4" t="s">
         <v>21</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E4">
@@ -557,7 +812,7 @@
       <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E5">
@@ -575,7 +830,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
         <v>27</v>
@@ -599,8 +854,1179 @@
         <v>13</v>
       </c>
     </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7">
+        <v>20</v>
+      </c>
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8">
+        <v>20</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9">
+        <v>20</v>
+      </c>
+      <c r="F9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10">
+        <v>20</v>
+      </c>
+      <c r="F10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11">
+        <v>23</v>
+      </c>
+      <c r="F11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12">
+        <v>23</v>
+      </c>
+      <c r="F12" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13">
+        <v>23</v>
+      </c>
+      <c r="F13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14">
+        <v>23</v>
+      </c>
+      <c r="F14" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15">
+        <v>23</v>
+      </c>
+      <c r="F15" t="s">
+        <v>45</v>
+      </c>
+      <c r="G15" t="s">
+        <v>12</v>
+      </c>
+      <c r="H15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16">
+        <v>28</v>
+      </c>
+      <c r="F16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" t="s">
+        <v>12</v>
+      </c>
+      <c r="H16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17">
+        <v>28</v>
+      </c>
+      <c r="F17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" t="s">
+        <v>12</v>
+      </c>
+      <c r="H17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" t="s">
+        <v>81</v>
+      </c>
+      <c r="C18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18">
+        <v>28</v>
+      </c>
+      <c r="F18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19">
+        <v>28</v>
+      </c>
+      <c r="F19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" t="s">
+        <v>25</v>
+      </c>
+      <c r="H19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20">
+        <v>28</v>
+      </c>
+      <c r="F20" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" t="s">
+        <v>25</v>
+      </c>
+      <c r="H20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C21" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21">
+        <v>28</v>
+      </c>
+      <c r="F21" t="s">
+        <v>46</v>
+      </c>
+      <c r="G21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E22">
+        <v>28</v>
+      </c>
+      <c r="F22" t="s">
+        <v>46</v>
+      </c>
+      <c r="G22" t="s">
+        <v>25</v>
+      </c>
+      <c r="H22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23">
+        <v>28</v>
+      </c>
+      <c r="F23" t="s">
+        <v>46</v>
+      </c>
+      <c r="G23" t="s">
+        <v>25</v>
+      </c>
+      <c r="H23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24">
+        <v>28</v>
+      </c>
+      <c r="F24" t="s">
+        <v>46</v>
+      </c>
+      <c r="G24" t="s">
+        <v>25</v>
+      </c>
+      <c r="H24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" t="s">
+        <v>87</v>
+      </c>
+      <c r="C25" t="s">
+        <v>67</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25">
+        <v>28</v>
+      </c>
+      <c r="F25" t="s">
+        <v>46</v>
+      </c>
+      <c r="G25" t="s">
+        <v>12</v>
+      </c>
+      <c r="H25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" t="s">
+        <v>88</v>
+      </c>
+      <c r="C26" t="s">
+        <v>67</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E26">
+        <v>18</v>
+      </c>
+      <c r="F26" t="s">
+        <v>46</v>
+      </c>
+      <c r="G26" t="s">
+        <v>12</v>
+      </c>
+      <c r="H26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E27">
+        <v>20</v>
+      </c>
+      <c r="F27" t="s">
+        <v>46</v>
+      </c>
+      <c r="G27" t="s">
+        <v>12</v>
+      </c>
+      <c r="H27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" t="s">
+        <v>90</v>
+      </c>
+      <c r="C28" t="s">
+        <v>67</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E28">
+        <v>25</v>
+      </c>
+      <c r="F28" t="s">
+        <v>46</v>
+      </c>
+      <c r="G28" t="s">
+        <v>12</v>
+      </c>
+      <c r="H28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" t="s">
+        <v>78</v>
+      </c>
+      <c r="C29" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E29">
+        <v>25</v>
+      </c>
+      <c r="F29" t="s">
+        <v>47</v>
+      </c>
+      <c r="G29" t="s">
+        <v>12</v>
+      </c>
+      <c r="H29" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" t="s">
+        <v>91</v>
+      </c>
+      <c r="C30" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E30">
+        <v>25</v>
+      </c>
+      <c r="F30" t="s">
+        <v>47</v>
+      </c>
+      <c r="G30" t="s">
+        <v>12</v>
+      </c>
+      <c r="H30" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" t="s">
+        <v>92</v>
+      </c>
+      <c r="C31" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E31">
+        <v>25</v>
+      </c>
+      <c r="F31" t="s">
+        <v>47</v>
+      </c>
+      <c r="G31" t="s">
+        <v>12</v>
+      </c>
+      <c r="H31" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>57</v>
+      </c>
+      <c r="B32" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E32">
+        <v>25</v>
+      </c>
+      <c r="F32" t="s">
+        <v>47</v>
+      </c>
+      <c r="G32" t="s">
+        <v>12</v>
+      </c>
+      <c r="H32" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>58</v>
+      </c>
+      <c r="B33" t="s">
+        <v>80</v>
+      </c>
+      <c r="C33" t="s">
+        <v>68</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E33">
+        <v>25</v>
+      </c>
+      <c r="F33" t="s">
+        <v>47</v>
+      </c>
+      <c r="G33" t="s">
+        <v>12</v>
+      </c>
+      <c r="H33" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" t="s">
+        <v>95</v>
+      </c>
+      <c r="C34" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E34">
+        <v>25</v>
+      </c>
+      <c r="F34" t="s">
+        <v>47</v>
+      </c>
+      <c r="G34" t="s">
+        <v>12</v>
+      </c>
+      <c r="H34" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35" t="s">
+        <v>96</v>
+      </c>
+      <c r="C35" t="s">
+        <v>68</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E35">
+        <v>25</v>
+      </c>
+      <c r="F35" t="s">
+        <v>47</v>
+      </c>
+      <c r="G35" t="s">
+        <v>25</v>
+      </c>
+      <c r="H35" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>60</v>
+      </c>
+      <c r="B36" t="s">
+        <v>97</v>
+      </c>
+      <c r="C36" t="s">
+        <v>68</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E36">
+        <v>20</v>
+      </c>
+      <c r="F36" t="s">
+        <v>47</v>
+      </c>
+      <c r="G36" t="s">
+        <v>25</v>
+      </c>
+      <c r="H36" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>60</v>
+      </c>
+      <c r="B37" t="s">
+        <v>98</v>
+      </c>
+      <c r="C37" t="s">
+        <v>68</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E37">
+        <v>22</v>
+      </c>
+      <c r="F37" t="s">
+        <v>47</v>
+      </c>
+      <c r="G37" t="s">
+        <v>25</v>
+      </c>
+      <c r="H37" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>60</v>
+      </c>
+      <c r="B38" t="s">
+        <v>99</v>
+      </c>
+      <c r="C38" t="s">
+        <v>68</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E38">
+        <v>20</v>
+      </c>
+      <c r="F38" t="s">
+        <v>47</v>
+      </c>
+      <c r="G38" t="s">
+        <v>25</v>
+      </c>
+      <c r="H38" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>60</v>
+      </c>
+      <c r="B39" t="s">
+        <v>100</v>
+      </c>
+      <c r="C39" t="s">
+        <v>17</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E39">
+        <v>21</v>
+      </c>
+      <c r="F39" t="s">
+        <v>47</v>
+      </c>
+      <c r="G39" t="s">
+        <v>25</v>
+      </c>
+      <c r="H39" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>60</v>
+      </c>
+      <c r="B40" t="s">
+        <v>93</v>
+      </c>
+      <c r="C40" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E40">
+        <v>19</v>
+      </c>
+      <c r="F40" t="s">
+        <v>10</v>
+      </c>
+      <c r="G40" t="s">
+        <v>25</v>
+      </c>
+      <c r="H40" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>60</v>
+      </c>
+      <c r="B41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C41" t="s">
+        <v>21</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E41">
+        <v>20</v>
+      </c>
+      <c r="F41" t="s">
+        <v>10</v>
+      </c>
+      <c r="G41" t="s">
+        <v>25</v>
+      </c>
+      <c r="H41" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>61</v>
+      </c>
+      <c r="B42" t="s">
+        <v>103</v>
+      </c>
+      <c r="C42" t="s">
+        <v>69</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E42">
+        <v>20</v>
+      </c>
+      <c r="F42" t="s">
+        <v>48</v>
+      </c>
+      <c r="G42" t="s">
+        <v>25</v>
+      </c>
+      <c r="H42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>61</v>
+      </c>
+      <c r="B43" t="s">
+        <v>104</v>
+      </c>
+      <c r="C43" t="s">
+        <v>69</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E43">
+        <v>20</v>
+      </c>
+      <c r="F43" t="s">
+        <v>48</v>
+      </c>
+      <c r="G43" t="s">
+        <v>25</v>
+      </c>
+      <c r="H43" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>61</v>
+      </c>
+      <c r="B44" t="s">
+        <v>105</v>
+      </c>
+      <c r="C44" t="s">
+        <v>69</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E44">
+        <v>20</v>
+      </c>
+      <c r="F44" t="s">
+        <v>48</v>
+      </c>
+      <c r="G44" t="s">
+        <v>25</v>
+      </c>
+      <c r="H44" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>61</v>
+      </c>
+      <c r="B45" t="s">
+        <v>107</v>
+      </c>
+      <c r="C45" t="s">
+        <v>70</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E45">
+        <v>22</v>
+      </c>
+      <c r="F45" t="s">
+        <v>49</v>
+      </c>
+      <c r="G45" t="s">
+        <v>19</v>
+      </c>
+      <c r="H45" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>62</v>
+      </c>
+      <c r="B46" t="s">
+        <v>106</v>
+      </c>
+      <c r="C46" t="s">
+        <v>70</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E46">
+        <v>20</v>
+      </c>
+      <c r="F46" t="s">
+        <v>49</v>
+      </c>
+      <c r="G46" t="s">
+        <v>19</v>
+      </c>
+      <c r="H46" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>63</v>
+      </c>
+      <c r="B47" t="s">
+        <v>108</v>
+      </c>
+      <c r="C47" t="s">
+        <v>71</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E47">
+        <v>20</v>
+      </c>
+      <c r="F47" t="s">
+        <v>50</v>
+      </c>
+      <c r="G47" t="s">
+        <v>19</v>
+      </c>
+      <c r="H47" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>63</v>
+      </c>
+      <c r="B48" t="s">
+        <v>109</v>
+      </c>
+      <c r="C48" t="s">
+        <v>71</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E48">
+        <v>22</v>
+      </c>
+      <c r="F48" t="s">
+        <v>50</v>
+      </c>
+      <c r="G48" t="s">
+        <v>19</v>
+      </c>
+      <c r="H48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>63</v>
+      </c>
+      <c r="B49" t="s">
+        <v>101</v>
+      </c>
+      <c r="C49" t="s">
+        <v>72</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E49">
+        <v>20</v>
+      </c>
+      <c r="F49" t="s">
+        <v>51</v>
+      </c>
+      <c r="G49" t="s">
+        <v>19</v>
+      </c>
+      <c r="H49" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>63</v>
+      </c>
+      <c r="B50" t="s">
+        <v>102</v>
+      </c>
+      <c r="C50" t="s">
+        <v>72</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E50">
+        <v>20</v>
+      </c>
+      <c r="F50" t="s">
+        <v>51</v>
+      </c>
+      <c r="G50" t="s">
+        <v>19</v>
+      </c>
+      <c r="H50" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>63</v>
+      </c>
+      <c r="B51" t="s">
+        <v>110</v>
+      </c>
+      <c r="C51" t="s">
+        <v>72</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E51">
+        <v>23</v>
+      </c>
+      <c r="F51" t="s">
+        <v>10</v>
+      </c>
+      <c r="G51" t="s">
+        <v>25</v>
+      </c>
+      <c r="H51" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="D6" twoDigitTextYear="1"/>
   </ignoredErrors>

</xml_diff>